<commit_message>
INTYGFV-13220: Adapted tests to new logic regarding measures. Fixed missing parameter indata for priority/order (excel)
</commit_message>
<xml_diff>
--- a/web/src/main/resources/SRS_PM_indata_2_2.xlsx
+++ b/web/src/main/resources/SRS_PM_indata_2_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Development/inera/intyg/srs/web/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A61E646-2C00-E843-A946-6FCEEAB2DF97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6CEA4A-8F09-F442-A41B-7D511914EA96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28600" yWindow="4240" windowWidth="20000" windowHeight="20140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11960" yWindow="1820" windowWidth="20000" windowHeight="20140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kodning av variabelnamn" sheetId="1" r:id="rId1"/>
@@ -1914,8 +1914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D150" sqref="D150"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3383,6 +3383,9 @@
       <c r="C100" t="s">
         <v>109</v>
       </c>
+      <c r="D100">
+        <v>2</v>
+      </c>
       <c r="E100" t="s">
         <v>110</v>
       </c>
@@ -3397,6 +3400,9 @@
       <c r="C101" t="s">
         <v>112</v>
       </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
       <c r="E101" t="s">
         <v>113</v>
       </c>
@@ -3467,6 +3473,9 @@
       <c r="C106" t="s">
         <v>109</v>
       </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
       <c r="E106" t="s">
         <v>110</v>
       </c>
@@ -3480,6 +3489,9 @@
       </c>
       <c r="C107" t="s">
         <v>112</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
       </c>
       <c r="E107" t="s">
         <v>113</v>
@@ -4140,9 +4152,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C232"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="A203" sqref="A203:XFD212"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.83203125" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>